<commit_message>
[ADD] CDUN ADM PERSONAL
</commit_message>
<xml_diff>
--- a/análisis/Casos de Uso Narrativos/CDUN - (Administrar Personal) Eliminar Hostel Worker.xlsx
+++ b/análisis/Casos de Uso Narrativos/CDUN - (Administrar Personal) Eliminar Hostel Worker.xlsx
@@ -1178,6 +1178,37 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1187,6 +1218,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1199,38 +1231,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1513,7 +1513,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:K34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
       <selection activeCell="C26" sqref="C26:I26"/>
     </sheetView>
   </sheetViews>
@@ -1531,97 +1531,97 @@
   <sheetData>
     <row r="1" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B2" s="52" t="s">
+      <c r="B2" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="38"/>
-      <c r="D2" s="53"/>
-      <c r="E2" s="36" t="s">
+      <c r="C2" s="20"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="53"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="21"/>
       <c r="I2" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B3" s="44" t="s">
+      <c r="B3" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="45"/>
-      <c r="D3" s="46"/>
-      <c r="E3" s="33" t="s">
+      <c r="C3" s="24"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="F3" s="33"/>
-      <c r="G3" s="33"/>
-      <c r="H3" s="33"/>
-      <c r="I3" s="34"/>
+      <c r="F3" s="26"/>
+      <c r="G3" s="26"/>
+      <c r="H3" s="26"/>
+      <c r="I3" s="27"/>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B4" s="44" t="s">
+      <c r="B4" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="45"/>
-      <c r="D4" s="46"/>
-      <c r="E4" s="33" t="s">
+      <c r="C4" s="24"/>
+      <c r="D4" s="25"/>
+      <c r="E4" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="F4" s="33"/>
-      <c r="G4" s="33"/>
-      <c r="H4" s="33"/>
-      <c r="I4" s="34"/>
+      <c r="F4" s="26"/>
+      <c r="G4" s="26"/>
+      <c r="H4" s="26"/>
+      <c r="I4" s="27"/>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B5" s="44" t="s">
+      <c r="B5" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="45"/>
-      <c r="D5" s="46"/>
+      <c r="C5" s="24"/>
+      <c r="D5" s="25"/>
       <c r="E5" s="3"/>
-      <c r="F5" s="47" t="s">
+      <c r="F5" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="G5" s="47"/>
-      <c r="H5" s="47"/>
-      <c r="I5" s="48"/>
+      <c r="G5" s="31"/>
+      <c r="H5" s="31"/>
+      <c r="I5" s="32"/>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B6" s="44" t="s">
+      <c r="B6" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="45"/>
-      <c r="D6" s="46"/>
-      <c r="E6" s="33" t="s">
+      <c r="C6" s="24"/>
+      <c r="D6" s="25"/>
+      <c r="E6" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="F6" s="33"/>
-      <c r="G6" s="33"/>
-      <c r="H6" s="33"/>
-      <c r="I6" s="34"/>
+      <c r="F6" s="26"/>
+      <c r="G6" s="26"/>
+      <c r="H6" s="26"/>
+      <c r="I6" s="27"/>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B7" s="44" t="s">
+      <c r="B7" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="45"/>
-      <c r="D7" s="46"/>
-      <c r="E7" s="33" t="s">
+      <c r="C7" s="24"/>
+      <c r="D7" s="25"/>
+      <c r="E7" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="F7" s="33"/>
-      <c r="G7" s="33"/>
-      <c r="H7" s="33"/>
-      <c r="I7" s="34"/>
+      <c r="F7" s="26"/>
+      <c r="G7" s="26"/>
+      <c r="H7" s="26"/>
+      <c r="I7" s="27"/>
     </row>
     <row r="8" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="49" t="s">
+      <c r="B8" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="50"/>
-      <c r="D8" s="51"/>
+      <c r="C8" s="34"/>
+      <c r="D8" s="35"/>
       <c r="E8" s="4" t="s">
         <v>28</v>
       </c>
@@ -1640,80 +1640,80 @@
     </row>
     <row r="9" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="10" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B10" s="29" t="s">
+      <c r="B10" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="30"/>
-      <c r="D10" s="30"/>
-      <c r="E10" s="30"/>
-      <c r="F10" s="30"/>
-      <c r="G10" s="30"/>
-      <c r="H10" s="30"/>
-      <c r="I10" s="31"/>
+      <c r="C10" s="37"/>
+      <c r="D10" s="37"/>
+      <c r="E10" s="37"/>
+      <c r="F10" s="37"/>
+      <c r="G10" s="37"/>
+      <c r="H10" s="37"/>
+      <c r="I10" s="38"/>
     </row>
     <row r="11" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="26" t="s">
+      <c r="B11" s="39" t="s">
         <v>30</v>
       </c>
-      <c r="C11" s="27"/>
-      <c r="D11" s="27"/>
-      <c r="E11" s="27"/>
-      <c r="F11" s="27"/>
-      <c r="G11" s="27"/>
-      <c r="H11" s="27"/>
-      <c r="I11" s="28"/>
+      <c r="C11" s="40"/>
+      <c r="D11" s="40"/>
+      <c r="E11" s="40"/>
+      <c r="F11" s="40"/>
+      <c r="G11" s="40"/>
+      <c r="H11" s="40"/>
+      <c r="I11" s="41"/>
     </row>
     <row r="12" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="13" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B13" s="29" t="s">
+      <c r="B13" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="30"/>
-      <c r="D13" s="30"/>
-      <c r="E13" s="30"/>
-      <c r="F13" s="30"/>
-      <c r="G13" s="30"/>
-      <c r="H13" s="30"/>
-      <c r="I13" s="31"/>
+      <c r="C13" s="37"/>
+      <c r="D13" s="37"/>
+      <c r="E13" s="37"/>
+      <c r="F13" s="37"/>
+      <c r="G13" s="37"/>
+      <c r="H13" s="37"/>
+      <c r="I13" s="38"/>
     </row>
     <row r="14" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="26" t="s">
+      <c r="B14" s="39" t="s">
         <v>31</v>
       </c>
-      <c r="C14" s="27"/>
-      <c r="D14" s="27"/>
-      <c r="E14" s="27"/>
-      <c r="F14" s="27"/>
-      <c r="G14" s="27"/>
-      <c r="H14" s="27"/>
-      <c r="I14" s="28"/>
+      <c r="C14" s="40"/>
+      <c r="D14" s="40"/>
+      <c r="E14" s="40"/>
+      <c r="F14" s="40"/>
+      <c r="G14" s="40"/>
+      <c r="H14" s="40"/>
+      <c r="I14" s="41"/>
     </row>
     <row r="15" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="16" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="41" t="s">
+      <c r="B16" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="C16" s="42"/>
-      <c r="D16" s="42"/>
-      <c r="E16" s="42"/>
-      <c r="F16" s="42"/>
-      <c r="G16" s="42"/>
-      <c r="H16" s="42"/>
-      <c r="I16" s="43"/>
+      <c r="C16" s="29"/>
+      <c r="D16" s="29"/>
+      <c r="E16" s="29"/>
+      <c r="F16" s="29"/>
+      <c r="G16" s="29"/>
+      <c r="H16" s="29"/>
+      <c r="I16" s="30"/>
     </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B17" s="6">
         <v>1</v>
       </c>
-      <c r="C17" s="35" t="s">
+      <c r="C17" s="42" t="s">
         <v>32</v>
       </c>
-      <c r="D17" s="36"/>
-      <c r="E17" s="37"/>
+      <c r="D17" s="22"/>
+      <c r="E17" s="43"/>
       <c r="F17" s="6"/>
-      <c r="G17" s="36"/>
-      <c r="H17" s="38"/>
-      <c r="I17" s="39"/>
+      <c r="G17" s="22"/>
+      <c r="H17" s="20"/>
+      <c r="I17" s="44"/>
     </row>
     <row r="18" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B18" s="16">
@@ -1727,11 +1727,11 @@
       <c r="F18" s="16">
         <v>3</v>
       </c>
-      <c r="G18" s="19" t="s">
+      <c r="G18" s="46" t="s">
         <v>34</v>
       </c>
-      <c r="H18" s="20"/>
-      <c r="I18" s="25"/>
+      <c r="H18" s="47"/>
+      <c r="I18" s="53"/>
       <c r="J18" s="17"/>
       <c r="K18" s="17"/>
     </row>
@@ -1739,232 +1739,202 @@
       <c r="B19" s="12">
         <v>4</v>
       </c>
-      <c r="C19" s="19" t="s">
+      <c r="C19" s="46" t="s">
         <v>35</v>
       </c>
-      <c r="D19" s="20"/>
-      <c r="E19" s="21"/>
+      <c r="D19" s="47"/>
+      <c r="E19" s="48"/>
       <c r="F19" s="12">
         <v>5</v>
       </c>
-      <c r="G19" s="22" t="s">
+      <c r="G19" s="50" t="s">
         <v>36</v>
       </c>
-      <c r="H19" s="23"/>
-      <c r="I19" s="24"/>
+      <c r="H19" s="51"/>
+      <c r="I19" s="52"/>
     </row>
     <row r="20" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B20" s="16">
         <v>6</v>
       </c>
-      <c r="C20" s="19" t="s">
+      <c r="C20" s="46" t="s">
         <v>37</v>
       </c>
-      <c r="D20" s="20"/>
-      <c r="E20" s="21"/>
+      <c r="D20" s="47"/>
+      <c r="E20" s="48"/>
       <c r="F20" s="16">
         <v>7</v>
       </c>
-      <c r="G20" s="19" t="s">
+      <c r="G20" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="H20" s="20"/>
-      <c r="I20" s="21"/>
+      <c r="H20" s="47"/>
+      <c r="I20" s="48"/>
     </row>
     <row r="21" spans="2:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B21" s="7">
         <v>8</v>
       </c>
-      <c r="C21" s="27" t="s">
+      <c r="C21" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="D21" s="40"/>
-      <c r="E21" s="28"/>
+      <c r="D21" s="45"/>
+      <c r="E21" s="41"/>
       <c r="F21" s="7"/>
-      <c r="G21" s="27"/>
-      <c r="H21" s="27"/>
-      <c r="I21" s="28"/>
+      <c r="G21" s="40"/>
+      <c r="H21" s="40"/>
+      <c r="I21" s="41"/>
     </row>
     <row r="22" spans="2:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B22" s="8"/>
       <c r="F22" s="8"/>
     </row>
     <row r="23" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B23" s="29" t="s">
+      <c r="B23" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="C23" s="30"/>
-      <c r="D23" s="30"/>
-      <c r="E23" s="30"/>
-      <c r="F23" s="30"/>
-      <c r="G23" s="30"/>
-      <c r="H23" s="30"/>
-      <c r="I23" s="31"/>
+      <c r="C23" s="37"/>
+      <c r="D23" s="37"/>
+      <c r="E23" s="37"/>
+      <c r="F23" s="37"/>
+      <c r="G23" s="37"/>
+      <c r="H23" s="37"/>
+      <c r="I23" s="38"/>
     </row>
     <row r="24" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B24" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="C24" s="33" t="s">
+      <c r="C24" s="26" t="s">
         <v>46</v>
       </c>
-      <c r="D24" s="33"/>
-      <c r="E24" s="33"/>
-      <c r="F24" s="33"/>
-      <c r="G24" s="33"/>
-      <c r="H24" s="33"/>
-      <c r="I24" s="34"/>
+      <c r="D24" s="26"/>
+      <c r="E24" s="26"/>
+      <c r="F24" s="26"/>
+      <c r="G24" s="26"/>
+      <c r="H24" s="26"/>
+      <c r="I24" s="27"/>
     </row>
     <row r="25" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B25" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="C25" s="19" t="s">
+      <c r="C25" s="46" t="s">
         <v>48</v>
       </c>
-      <c r="D25" s="20"/>
-      <c r="E25" s="20"/>
-      <c r="F25" s="20"/>
-      <c r="G25" s="20"/>
-      <c r="H25" s="20"/>
-      <c r="I25" s="21"/>
+      <c r="D25" s="47"/>
+      <c r="E25" s="47"/>
+      <c r="F25" s="47"/>
+      <c r="G25" s="47"/>
+      <c r="H25" s="47"/>
+      <c r="I25" s="48"/>
     </row>
     <row r="26" spans="2:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B26" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="C26" s="27" t="s">
+      <c r="C26" s="40" t="s">
         <v>47</v>
       </c>
-      <c r="D26" s="27"/>
-      <c r="E26" s="27"/>
-      <c r="F26" s="27"/>
-      <c r="G26" s="27"/>
-      <c r="H26" s="27"/>
-      <c r="I26" s="28"/>
+      <c r="D26" s="40"/>
+      <c r="E26" s="40"/>
+      <c r="F26" s="40"/>
+      <c r="G26" s="40"/>
+      <c r="H26" s="40"/>
+      <c r="I26" s="41"/>
     </row>
     <row r="27" spans="2:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="28" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B28" s="29" t="s">
+      <c r="B28" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="C28" s="30"/>
-      <c r="D28" s="30"/>
-      <c r="E28" s="30"/>
-      <c r="F28" s="30"/>
-      <c r="G28" s="30"/>
-      <c r="H28" s="30"/>
-      <c r="I28" s="31"/>
+      <c r="C28" s="37"/>
+      <c r="D28" s="37"/>
+      <c r="E28" s="37"/>
+      <c r="F28" s="37"/>
+      <c r="G28" s="37"/>
+      <c r="H28" s="37"/>
+      <c r="I28" s="38"/>
     </row>
     <row r="29" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B29" s="32" t="s">
+      <c r="B29" s="49" t="s">
         <v>15</v>
       </c>
-      <c r="C29" s="33"/>
-      <c r="D29" s="33"/>
+      <c r="C29" s="26"/>
+      <c r="D29" s="26"/>
       <c r="E29" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="F29" s="33" t="s">
+      <c r="F29" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="G29" s="33"/>
-      <c r="H29" s="33" t="s">
+      <c r="G29" s="26"/>
+      <c r="H29" s="26" t="s">
         <v>44</v>
       </c>
-      <c r="I29" s="34"/>
+      <c r="I29" s="27"/>
     </row>
     <row r="30" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B30" s="32" t="s">
+      <c r="B30" s="49" t="s">
         <v>17</v>
       </c>
-      <c r="C30" s="33"/>
-      <c r="D30" s="33"/>
+      <c r="C30" s="26"/>
+      <c r="D30" s="26"/>
       <c r="E30" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="F30" s="33" t="s">
+      <c r="F30" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="G30" s="33"/>
-      <c r="H30" s="33" t="s">
+      <c r="G30" s="26"/>
+      <c r="H30" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="I30" s="34"/>
+      <c r="I30" s="27"/>
     </row>
     <row r="31" spans="2:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="26" t="s">
+      <c r="B31" s="39" t="s">
         <v>19</v>
       </c>
-      <c r="C31" s="27"/>
-      <c r="D31" s="27"/>
+      <c r="C31" s="40"/>
+      <c r="D31" s="40"/>
       <c r="E31" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="F31" s="27" t="s">
+      <c r="F31" s="40" t="s">
         <v>20</v>
       </c>
-      <c r="G31" s="27"/>
-      <c r="H31" s="27" t="s">
+      <c r="G31" s="40"/>
+      <c r="H31" s="40" t="s">
         <v>44</v>
       </c>
-      <c r="I31" s="28"/>
+      <c r="I31" s="41"/>
     </row>
     <row r="32" spans="2:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="33" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B33" s="29" t="s">
+      <c r="B33" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="C33" s="30"/>
-      <c r="D33" s="30"/>
-      <c r="E33" s="30"/>
-      <c r="F33" s="30"/>
-      <c r="G33" s="30"/>
-      <c r="H33" s="30"/>
-      <c r="I33" s="31"/>
+      <c r="C33" s="37"/>
+      <c r="D33" s="37"/>
+      <c r="E33" s="37"/>
+      <c r="F33" s="37"/>
+      <c r="G33" s="37"/>
+      <c r="H33" s="37"/>
+      <c r="I33" s="38"/>
     </row>
     <row r="34" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="26"/>
-      <c r="C34" s="27"/>
-      <c r="D34" s="27"/>
-      <c r="E34" s="27"/>
-      <c r="F34" s="27"/>
-      <c r="G34" s="27"/>
-      <c r="H34" s="27"/>
-      <c r="I34" s="28"/>
+      <c r="B34" s="39"/>
+      <c r="C34" s="40"/>
+      <c r="D34" s="40"/>
+      <c r="E34" s="40"/>
+      <c r="F34" s="40"/>
+      <c r="G34" s="40"/>
+      <c r="H34" s="40"/>
+      <c r="I34" s="41"/>
     </row>
   </sheetData>
   <mergeCells count="43">
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="E2:H2"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="E3:I3"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="E4:I4"/>
-    <mergeCell ref="B16:I16"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="F5:I5"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="E6:I6"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="E7:I7"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="B10:I10"/>
-    <mergeCell ref="B11:I11"/>
-    <mergeCell ref="B13:I13"/>
-    <mergeCell ref="B14:I14"/>
-    <mergeCell ref="C17:E17"/>
-    <mergeCell ref="G17:I17"/>
-    <mergeCell ref="C21:E21"/>
-    <mergeCell ref="G21:I21"/>
-    <mergeCell ref="B23:I23"/>
-    <mergeCell ref="C20:E20"/>
-    <mergeCell ref="G20:I20"/>
-    <mergeCell ref="B33:I33"/>
-    <mergeCell ref="B34:I34"/>
-    <mergeCell ref="B30:D30"/>
-    <mergeCell ref="F30:G30"/>
-    <mergeCell ref="H30:I30"/>
     <mergeCell ref="C25:I25"/>
     <mergeCell ref="C19:E19"/>
     <mergeCell ref="G19:I19"/>
@@ -1978,6 +1948,36 @@
     <mergeCell ref="B29:D29"/>
     <mergeCell ref="F29:G29"/>
     <mergeCell ref="H29:I29"/>
+    <mergeCell ref="B33:I33"/>
+    <mergeCell ref="B34:I34"/>
+    <mergeCell ref="B30:D30"/>
+    <mergeCell ref="F30:G30"/>
+    <mergeCell ref="H30:I30"/>
+    <mergeCell ref="C17:E17"/>
+    <mergeCell ref="G17:I17"/>
+    <mergeCell ref="C21:E21"/>
+    <mergeCell ref="G21:I21"/>
+    <mergeCell ref="B23:I23"/>
+    <mergeCell ref="C20:E20"/>
+    <mergeCell ref="G20:I20"/>
+    <mergeCell ref="B16:I16"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="F5:I5"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="E6:I6"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="E7:I7"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="B10:I10"/>
+    <mergeCell ref="B11:I11"/>
+    <mergeCell ref="B13:I13"/>
+    <mergeCell ref="B14:I14"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="E2:H2"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="E3:I3"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="E4:I4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>